<commit_message>
Drag & Drop Adaption
</commit_message>
<xml_diff>
--- a/Docs/stundenliste_manuel.xlsx
+++ b/Docs/stundenliste_manuel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Manuel Seywald</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Drag&amp;Drop angepasst ("natürlicheres Steinelegen")</t>
+  </si>
+  <si>
+    <t>Drag&amp;Drop angepasst. Versuch eine "SteineVorschau" einzubauen</t>
+  </si>
+  <si>
+    <t>Drag&amp;Drop angepasst. Preview</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -172,6 +178,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -452,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -634,14 +642,36 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="5">
+        <v>42513</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B18" s="1">
-        <f>SUM(B3:B17)</f>
-        <v>34.5</v>
+      <c r="A18" s="5">
+        <v>42514</v>
+      </c>
+      <c r="B18" s="8">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B20" s="1">
+        <f>SUM(B3:B18)</f>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring - Movement Buttons
Looks ugly right now, because much duplicate code. But works :+1:
</commit_message>
<xml_diff>
--- a/Docs/stundenliste_manuel.xlsx
+++ b/Docs/stundenliste_manuel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingSeybro\Documents\GitHub\se2blokus\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingSeybro\Dropbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9855" windowHeight="3135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9857" windowHeight="3137"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Manuel Seywald</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Drehen soweit fertig. Brauchen halt noch einen schönen Button</t>
+  </si>
+  <si>
+    <t>Funktion, ob noch Spielzüge möglich sind - Rohfassung</t>
+  </si>
+  <si>
+    <t>Funktion überarbeitet, neue Idee, wird noch umgesetzt</t>
+  </si>
+  <si>
+    <t>Refactoring von Bewegungsbuttons von Markus und teaming mit Tobias</t>
   </si>
 </sst>
 </file>
@@ -199,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -212,6 +221,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -492,23 +502,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="87.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -519,7 +529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>42464</v>
       </c>
@@ -530,7 +540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="5">
         <v>42471</v>
       </c>
@@ -541,7 +551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="5">
         <v>42477</v>
       </c>
@@ -552,7 +562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="5">
         <v>42478</v>
       </c>
@@ -563,7 +573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="5">
         <v>42484</v>
       </c>
@@ -574,7 +584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="5">
         <v>42486</v>
       </c>
@@ -585,7 +595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="5">
         <v>42492</v>
       </c>
@@ -596,7 +606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="5">
         <v>42493</v>
       </c>
@@ -607,7 +617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>42497</v>
       </c>
@@ -618,7 +628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
         <v>42498</v>
       </c>
@@ -629,7 +639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="5">
         <v>42499</v>
       </c>
@@ -640,7 +650,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="5">
         <v>42500</v>
       </c>
@@ -651,7 +661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="5">
         <v>42506</v>
       </c>
@@ -662,7 +672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="5">
         <v>42511</v>
       </c>
@@ -673,7 +683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="5">
         <v>42513</v>
       </c>
@@ -684,7 +694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="5">
         <v>42514</v>
       </c>
@@ -695,7 +705,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="5">
         <v>42515</v>
       </c>
@@ -706,7 +716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="10">
         <v>42516</v>
       </c>
@@ -717,7 +727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="9">
         <v>42517</v>
       </c>
@@ -728,10 +738,48 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
-        <f>SUM(B3:B21)</f>
-        <v>52.5</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" s="9">
+        <v>42518</v>
+      </c>
+      <c r="B22" s="11">
+        <v>3</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" s="9">
+        <v>42519</v>
+      </c>
+      <c r="B23" s="11">
+        <v>1</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="9">
+        <v>42520</v>
+      </c>
+      <c r="B24" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" s="9"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B26" s="1">
+        <f>SUM(B3:B24)</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AnyTurnsLeft angepasst + BugFixing
Funktion müsste performanter sein und funktioniert prinzipiell (ohne
ausgiebiges Testen)
Ein Bug wurde mit Daniel gefixed, Steine wurden übermalt bei "rechts",
"runter", "links" Buttons
</commit_message>
<xml_diff>
--- a/Docs/stundenliste_manuel.xlsx
+++ b/Docs/stundenliste_manuel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9857" windowHeight="3137"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9855" windowHeight="3135"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Manuel Seywald</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Funktion die überprüft ob noch Spielzüge möglich sind - Rohfassung &amp; Punktestand mitzählen</t>
+  </si>
+  <si>
+    <t>Funktion die überprüft… überarbeitet (Performanter, noch nicht ausgiebig getestet), BugFixing</t>
   </si>
 </sst>
 </file>
@@ -131,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -196,11 +199,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -213,6 +227,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -495,21 +510,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="87.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -520,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>42464</v>
       </c>
@@ -531,7 +546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>42471</v>
       </c>
@@ -542,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>42477</v>
       </c>
@@ -553,7 +568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>42478</v>
       </c>
@@ -564,7 +579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>42484</v>
       </c>
@@ -575,7 +590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>42486</v>
       </c>
@@ -586,7 +601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>42492</v>
       </c>
@@ -597,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>42493</v>
       </c>
@@ -608,7 +623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>42497</v>
       </c>
@@ -619,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>42498</v>
       </c>
@@ -630,7 +645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>42499</v>
       </c>
@@ -641,7 +656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>42500</v>
       </c>
@@ -652,7 +667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>42506</v>
       </c>
@@ -663,7 +678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>42511</v>
       </c>
@@ -674,7 +689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>42513</v>
       </c>
@@ -685,7 +700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>42514</v>
       </c>
@@ -696,7 +711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>42515</v>
       </c>
@@ -707,7 +722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>42516</v>
       </c>
@@ -718,7 +733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>42517</v>
       </c>
@@ -729,7 +744,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>42518</v>
       </c>
@@ -740,7 +755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>42519</v>
       </c>
@@ -751,7 +766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>42520</v>
       </c>
@@ -762,7 +777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>42521</v>
       </c>
@@ -773,20 +788,26 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>42523</v>
+      </c>
+      <c r="B26" s="12">
+        <v>4</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
-        <f>SUM(B3:B25)</f>
-        <v>65.5</v>
+        <f>SUM(B3:B26)</f>
+        <v>69.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to fix bugs for left and up movement
</commit_message>
<xml_diff>
--- a/Docs/stundenliste_manuel.xlsx
+++ b/Docs/stundenliste_manuel.xlsx
@@ -128,7 +128,7 @@
     <t>Versuch AreTurnsLeft performanter zu machen | SplashScreen für unterschiedliche Bildschirmgrößen</t>
   </si>
   <si>
-    <t>Kleine Änderungen bei den Tests</t>
+    <t>Kleine Änderungen bei den Tests + Versuch Bugs zu fixen</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -915,7 +915,7 @@
         <v>42536</v>
       </c>
       <c r="B33" s="14">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>34</v>
@@ -929,7 +929,7 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B35" s="1">
         <f>SUM(B3:B33)</f>
-        <v>93</v>
+        <v>95.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AreTurnsLeft in Netzwerkkomm integriert
Wenn ein Spieler keine Züge mehr hat, wie kann ich dann zum nächsten
springen??
Ich hab versucht noch einmal isItMyTurn() aufzurufen, hat aber nicht
geklappt :(
</commit_message>
<xml_diff>
--- a/Docs/stundenliste_manuel.xlsx
+++ b/Docs/stundenliste_manuel.xlsx
@@ -128,7 +128,7 @@
     <t>Versuch AreTurnsLeft performanter zu machen | SplashScreen für unterschiedliche Bildschirmgrößen</t>
   </si>
   <si>
-    <t>Kleine Änderungen bei den Tests + Versuch Bugs zu fixen</t>
+    <t>Kleine Änderungen bei den Tests + Versuch Bugs zu fixen + AreTurnsLeft in Netzwerkkomm. Integriert</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -242,22 +242,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -272,7 +261,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -556,7 +544,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -867,57 +855,57 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" s="9">
+      <c r="A29" s="5">
         <v>42530</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="8">
         <v>3</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="9">
+      <c r="A30" s="5">
         <v>42531</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="8">
         <v>3</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" s="9">
+      <c r="A31" s="5">
         <v>42532</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="8">
         <v>2.5</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" s="9">
+      <c r="A32" s="5">
         <v>42535</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="8">
         <v>5.5</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" s="9">
+      <c r="A33" s="5">
         <v>42536</v>
       </c>
-      <c r="B33" s="14">
-        <v>4</v>
-      </c>
-      <c r="C33" s="14" t="s">
+      <c r="B33" s="8">
+        <v>6</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -929,7 +917,7 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B35" s="1">
         <f>SUM(B3:B33)</f>
-        <v>95.5</v>
+        <v>97.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>